<commit_message>
se grega en la platilla activación históricos otros campos
</commit_message>
<xml_diff>
--- a/plantillas/activacion.xlsx
+++ b/plantillas/activacion.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\gestoroperaciones\plantillas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="18915" windowHeight="10545"/>
   </bookViews>
@@ -11,12 +16,15 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>PEDIDO</t>
   </si>
@@ -88,25 +96,26 @@
   </si>
   <si>
     <t>FECHA_GESTION</t>
+  </si>
+  <si>
+    <t>FECHA_EXPORTE</t>
+  </si>
+  <si>
+    <t>HORA_EXPORTE</t>
+  </si>
+  <si>
+    <t>HORA_GESTION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -134,14 +143,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -152,8 +160,28 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Hoja1"/>
+      <sheetName val="Hoja2"/>
+      <sheetName val="Hoja3"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -199,7 +227,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -232,9 +260,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -267,6 +312,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -443,24 +505,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -498,29 +567,51 @@
         <v>14</v>
       </c>
       <c r="M1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M2" s="4"/>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2"/>
+      <c r="B2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Hoja2!$B$1:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L1048576</xm:sqref>
+          <xm:sqref>L3:L1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Hoja2!$A$1:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I1048576</xm:sqref>
+          <xm:sqref>I3:I1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[Formato.xlsx]Hoja2!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[Formato.xlsx]Hoja2!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>L2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
grega en la platilla activación históricos otros campos
</commit_message>
<xml_diff>
--- a/plantillas/activacion.xlsx
+++ b/plantillas/activacion.xlsx
@@ -14,17 +14,16 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterate="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>PEDIDO</t>
   </si>
@@ -105,6 +104,9 @@
   </si>
   <si>
     <t>HORA_GESTION</t>
+  </si>
+  <si>
+    <t>FENIX</t>
   </si>
 </sst>
 </file>
@@ -507,7 +509,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -588,13 +592,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Hoja2!$B$1:$B$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>L3:L1048576</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Hoja2!$A$1:$A$9</xm:f>
@@ -603,15 +601,15 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[Formato.xlsx]Hoja2!#REF!</xm:f>
+            <xm:f>Hoja2!$A:$A</xm:f>
           </x14:formula1>
           <xm:sqref>I2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[Formato.xlsx]Hoja2!#REF!</xm:f>
+            <xm:f>Hoja2!$B$1:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>L2</xm:sqref>
+          <xm:sqref>L2:L1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -623,9 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -657,6 +653,9 @@
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -681,16 +680,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>